<commit_message>
improved log4j and screen shots name
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anilkumar06\workspace\AmazonBackup\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anilkumar06\workspace\AmazonAutomation\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB1EB1-75CB-4ACD-83DE-7F33312B8895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5920BC-B75F-4936-BB9C-3CFB99B4D4A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Runmode</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Ndae10606</t>
   </si>
   <si>
-    <t>Oldest</t>
-  </si>
-  <si>
-    <t>sortText</t>
-  </si>
-  <si>
-    <t>couponSortTest</t>
-  </si>
-  <si>
     <t>categorySelectTest</t>
   </si>
   <si>
@@ -80,12 +71,6 @@
     <t>productAddtoCartTest</t>
   </si>
   <si>
-    <t>couponCategoryTest</t>
-  </si>
-  <si>
-    <t>categoryText</t>
-  </si>
-  <si>
     <t>validUserLoginLogoutTest</t>
   </si>
   <si>
@@ -99,6 +84,15 @@
   </si>
   <si>
     <t>boAt BassHeads 100 in-Ear Headphones with Mic (White)</t>
+  </si>
+  <si>
+    <t>dealsCategoryTest</t>
+  </si>
+  <si>
+    <t>dealsCategory</t>
+  </si>
+  <si>
+    <t>Books</t>
   </si>
 </sst>
 </file>
@@ -434,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,7 +445,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,7 +478,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -517,7 +511,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -525,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -533,15 +527,20 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -549,73 +548,44 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
+      <c r="B20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>